<commit_message>
change autofit call to be based per column
</commit_message>
<xml_diff>
--- a/packages/jsreport-xlsx/test/cols-autofit.xlsx
+++ b/packages/jsreport-xlsx/test/cols-autofit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/jsreport/jsreport/packages/jsreport-xlsx/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67D32B5-3E57-D443-9C17-89FD2CD009B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A969EB4D-0250-8548-B62F-E211E0A1714D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="2640" windowWidth="28040" windowHeight="17440" xr2:uid="{797EC867-59E6-3440-8685-3B2E92735B12}"/>
   </bookViews>
@@ -63,6 +63,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D77B34B7-3E50-A348-BE67-0AE7E9E734C0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>BORIS MATOS:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>{{xlsxColAutofit}}</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -92,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +153,12 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -462,7 +501,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>